<commit_message>
add txt preprocessing step
</commit_message>
<xml_diff>
--- a/output/trauma_data_audio_data.xlsx
+++ b/output/trauma_data_audio_data.xlsx
@@ -715,17 +715,17 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fall from height</t>
+          <t>fall from height</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Multiple fractures, internal bleeding, spinal injury</t>
+          <t>Fracture, Internal Bleeding</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>STAT trauma activation for 32-year-old female high fall victim. Multiple fractures including femur, pelvis, spine. Internal bleeding suspected. Blood pressure dropping. Immediate trauma team activation required.</t>
+          <t>Trauma activation for 32-year-old F with fall from height. Injuries: Fracture, Internal Bleeding. Trauma team activation required.</t>
         </is>
       </c>
     </row>
@@ -1099,17 +1099,17 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Motor vehicle accident</t>
+          <t>motor vehicle accident</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Head injury, chest trauma, rib fractures</t>
+          <t>Head Injury, Chest Trauma, Fracture, Rib Fracture, Skull Fracture</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>STAT trauma activation for 25-year-old male MVA victim with head injury and chest trauma. Patient unconscious, intubated, stable vitals. Immediate trauma team activation required.</t>
+          <t>Trauma activation for 25-year-old M with motor vehicle accident. Injuries: Head Injury, Chest Trauma, Fracture, Rib Fracture, Skull Fracture. Trauma team activation required.</t>
         </is>
       </c>
     </row>

</xml_diff>